<commit_message>
added nas net 12 epochs results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Inception V3</t>
   </si>
@@ -34,6 +34,12 @@
     <t>30 epochs</t>
   </si>
   <si>
+    <t>﻿</t>
+  </si>
+  <si>
+    <t>accuracy test: 0.9481096863746643</t>
+  </si>
+  <si>
     <t>Nas net</t>
   </si>
   <si>
@@ -48,17 +54,69 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFDCDDDE"/>
+      <name val="Whitney"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -78,21 +136,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -106,6 +181,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -113,94 +203,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,13 +239,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,19 +353,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,139 +407,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,6 +424,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -434,31 +470,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,17 +503,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -498,17 +510,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,156 +529,162 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -988,13 +1006,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:C12"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="15.7" customWidth="1"/>
     <col min="2" max="2" width="21.6" customWidth="1"/>
@@ -1031,22 +1049,30 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6">
         <v>0.974425494670867</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" ht="16.5" spans="5:5">
+      <c r="E7" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>0.960711658000946</v>
@@ -1054,9 +1080,11 @@
     </row>
     <row r="10" spans="2:3">
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.948109686374664</v>
+      </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">

</xml_diff>

<commit_message>
added inception v3 results for 25 epochs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Inception V3</t>
   </si>
   <si>
     <t>accuracy</t>
+  </si>
+  <si>
+    <t>10 epochs</t>
   </si>
   <si>
     <t>15 epochs</t>
@@ -31,19 +34,16 @@
     <t>25 epochs</t>
   </si>
   <si>
-    <t>30 epochs</t>
+    <t>﻿</t>
   </si>
   <si>
-    <t>﻿</t>
+    <t>30 epochs</t>
   </si>
   <si>
     <t>accuracy test: 0.9481096863746643</t>
   </si>
   <si>
     <t>Nas net</t>
-  </si>
-  <si>
-    <t>10 epochs</t>
   </si>
   <si>
     <t>12 epochs</t>
@@ -55,9 +55,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -83,22 +83,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -112,6 +97,90 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -121,7 +190,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -136,83 +205,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,19 +233,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,163 +383,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,6 +424,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -446,7 +455,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -466,22 +475,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,170 +507,166 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -674,11 +674,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -1006,10 +1009,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -1031,74 +1034,86 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>0.959970355033874</v>
-      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.975537419319152</v>
+        <v>0.959970355033874</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5">
+        <v>0.975537419319152</v>
+      </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>0.974425494670867</v>
+      <c r="C6" s="2">
+        <v>0.977020025253295</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" ht="16.5" spans="5:5">
-      <c r="E7" s="3" t="s">
+    <row r="7" ht="16.5" spans="2:5">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
+      <c r="C7">
+        <v>0.974425494670867</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="8" spans="2:2">
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
         <v>9</v>
-      </c>
-      <c r="C9">
-        <v>0.960711658000946</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.948109686374664</v>
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0.960711658000946</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>0.953669369220733</v>
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.948109686374664</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12">
+        <v>0.953669369220733</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
         <v>0.958858430385589</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added inception v3 results for 10 ehochepochs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -54,10 +54,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -83,7 +83,82 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -99,26 +174,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -126,14 +195,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -142,15 +203,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -158,61 +210,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,6 +233,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -245,175 +251,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,15 +424,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -451,11 +442,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -490,17 +487,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -529,121 +529,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -652,19 +652,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -678,13 +678,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1034,7 +1034,9 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>0.958117127418518</v>
+      </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
@@ -1091,7 +1093,7 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>0.948109686374664</v>
       </c>
     </row>
@@ -1107,7 +1109,7 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" t="s">

</xml_diff>

<commit_message>
added nas net results for 20 epochs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -54,8 +54,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -74,9 +74,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -84,36 +90,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,21 +103,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -150,15 +111,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,53 +203,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,7 +227,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,175 +371,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,32 +421,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -487,20 +469,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,157 +503,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -682,9 +676,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1012,7 +1003,7 @@
   <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -1058,7 +1049,7 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.977020025253295</v>
       </c>
       <c r="E6" t="s">
@@ -1072,7 +1063,7 @@
       <c r="C7">
         <v>0.974425494670867</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1093,7 +1084,7 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>0.948109686374664</v>
       </c>
     </row>
@@ -1109,7 +1100,9 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2">
+        <v>0.960340976715087</v>
+      </c>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" t="s">

</xml_diff>

<commit_message>
added results for without validation split, inception v3, 5 epochs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8445"/>
+    <workbookView windowWidth="20385" windowHeight="8475" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="with_validation" sheetId="1" r:id="rId1"/>
+    <sheet name="without_validation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Inception V3</t>
   </si>
@@ -47,6 +48,21 @@
   </si>
   <si>
     <t>12 epochs</t>
+  </si>
+  <si>
+    <t>training accuracy</t>
+  </si>
+  <si>
+    <t>training loss</t>
+  </si>
+  <si>
+    <t>validation accuracy</t>
+  </si>
+  <si>
+    <t>validation loss</t>
+  </si>
+  <si>
+    <t>5 epochs</t>
   </si>
 </sst>
 </file>
@@ -54,10 +70,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -74,24 +90,27 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -103,6 +122,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -111,6 +137,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -121,75 +184,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,15 +214,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,25 +243,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,157 +411,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,6 +434,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -433,8 +458,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -495,15 +520,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -523,118 +539,118 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -643,36 +659,33 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -1002,8 +1015,8 @@
   <sheetPr/>
   <dimension ref="B2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -1063,7 +1076,7 @@
       <c r="C7">
         <v>0.974425494670867</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1100,7 +1113,7 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>0.960340976715087</v>
       </c>
     </row>
@@ -1111,6 +1124,113 @@
       <c r="C14">
         <v>0.958858430385589</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="C6:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="6"/>
+  <cols>
+    <col min="3" max="3" width="12.1" customWidth="1"/>
+    <col min="4" max="4" width="20.7" customWidth="1"/>
+    <col min="5" max="5" width="14.2" customWidth="1"/>
+    <col min="6" max="6" width="15.8" customWidth="1"/>
+    <col min="7" max="7" width="17.1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" ht="13" customHeight="1" spans="3:7">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>0.9893</v>
+      </c>
+      <c r="E7">
+        <v>0.0367</v>
+      </c>
+      <c r="F7">
+        <v>0.9907</v>
+      </c>
+      <c r="G7">
+        <v>0.0458</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4">
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="3:3">
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="4:4">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="14" spans="3:3">
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7">
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>0.9869</v>
+      </c>
+      <c r="E15">
+        <v>0.0401</v>
+      </c>
+      <c r="F15">
+        <v>0.9867</v>
+      </c>
+      <c r="G15">
+        <v>0.0498</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3">
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added results for without validation split, with graphs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8475" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="with_validation" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Inception V3</t>
   </si>
@@ -70,10 +70,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -98,6 +98,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -106,11 +137,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -122,15 +175,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -138,7 +192,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -152,7 +213,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -160,75 +228,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,37 +243,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,145 +387,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,9 +439,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -455,11 +457,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -494,6 +502,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -508,179 +534,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -688,10 +688,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -873,7 +873,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -897,9 +897,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -923,7 +923,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -976,7 +976,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1001,7 +1001,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1019,10 +1019,10 @@
       <selection activeCell="B1" sqref="B1:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="15.7" customWidth="1"/>
-    <col min="2" max="2" width="21.6" customWidth="1"/>
+    <col min="1" max="1" width="15.7" customWidth="true"/>
+    <col min="2" max="2" width="21.6" customWidth="true"/>
     <col min="3" max="3" width="12.5"/>
   </cols>
   <sheetData>
@@ -1069,7 +1069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" ht="16.5" spans="2:5">
+    <row r="7" ht="17.25" spans="2:5">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1134,22 +1134,22 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C6:G18"/>
+  <dimension ref="C6:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="6"/>
   <cols>
-    <col min="3" max="3" width="12.1" customWidth="1"/>
-    <col min="4" max="4" width="20.7" customWidth="1"/>
-    <col min="5" max="5" width="14.2" customWidth="1"/>
-    <col min="6" max="6" width="15.8" customWidth="1"/>
-    <col min="7" max="7" width="17.1" customWidth="1"/>
+    <col min="3" max="3" width="12.1" customWidth="true"/>
+    <col min="4" max="4" width="20.7" customWidth="true"/>
+    <col min="5" max="5" width="14.2" customWidth="true"/>
+    <col min="6" max="6" width="15.8" customWidth="true"/>
+    <col min="7" max="7" width="17.1" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="6" ht="13" customHeight="1" spans="3:7">
+    <row r="6" ht="13" customHeight="true" spans="3:7">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -1183,54 +1183,115 @@
         <v>0.0458</v>
       </c>
     </row>
-    <row r="8" spans="3:4">
+    <row r="8" spans="3:7">
       <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="3:3">
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="4:4">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="14" spans="3:3">
-      <c r="C14" t="s">
+      <c r="D8" s="1">
+        <v>0.9978</v>
+      </c>
+      <c r="E8">
+        <v>0.0074</v>
+      </c>
+      <c r="F8">
+        <v>0.9907</v>
+      </c>
+      <c r="G8">
+        <v>0.0442</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="3:7">
-      <c r="C15" t="s">
+    <row r="12" spans="3:7">
+      <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="D15">
+      <c r="D12">
         <v>0.9869</v>
       </c>
-      <c r="E15">
+      <c r="E12">
         <v>0.0401</v>
       </c>
-      <c r="F15">
+      <c r="F12">
         <v>0.9867</v>
       </c>
-      <c r="G15">
+      <c r="G12">
         <v>0.0498</v>
       </c>
     </row>
-    <row r="16" spans="3:3">
-      <c r="C16" t="s">
+    <row r="13" spans="3:7">
+      <c r="C13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" s="1"/>
+      <c r="D13">
+        <v>0.9945</v>
+      </c>
+      <c r="E13">
+        <v>0.0187</v>
+      </c>
+      <c r="F13">
+        <v>0.9863</v>
+      </c>
+      <c r="G13">
+        <v>0.0655</v>
+      </c>
+    </row>
+    <row r="15" spans="4:4">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="18" spans="4:7">
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0.9893</v>
+      </c>
+      <c r="E19">
+        <v>0.0367</v>
+      </c>
+      <c r="F19">
+        <v>0.9907</v>
+      </c>
+      <c r="G19">
+        <v>0.0458</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>0.9869</v>
+      </c>
+      <c r="E20">
+        <v>0.0401</v>
+      </c>
+      <c r="F20">
+        <v>0.9867</v>
+      </c>
+      <c r="G20">
+        <v>0.0498</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>